<commit_message>
Atualizei a aba de Pessoa Logada
</commit_message>
<xml_diff>
--- a/Backlog_do_Projeto (1).xlsx
+++ b/Backlog_do_Projeto (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silva\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silva\Documents\Entregaveis sprint 2\Projeto-Sprint-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B465C59B-D6A6-40FF-9468-092729D72A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5131EFF0-062A-4259-850D-E6909090011C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9B2F8E2-95A5-4C11-9E48-BCDD2490E4AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -127,19 +127,13 @@
   </si>
   <si>
     <t>Ordem de Excução</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint </t>
-  </si>
-  <si>
-    <t>Sprint02 16/04/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +160,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -182,19 +195,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor rgb="FFAEABAB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -248,17 +261,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEF45EA-656C-4129-B945-0C7E43FB7173}">
-  <dimension ref="B3:G25"/>
+  <dimension ref="B3:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,38 +607,34 @@
     <col min="3" max="3" width="110.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+    </row>
+    <row r="4" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10">
@@ -625,18 +643,15 @@
       <c r="F4" s="10">
         <v>1</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+    </row>
+    <row r="5" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="10">
@@ -645,16 +660,15 @@
       <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="6" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="10">
@@ -663,16 +677,15 @@
       <c r="F6" s="10">
         <v>3</v>
       </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
+    </row>
+    <row r="7" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="10">
@@ -681,16 +694,15 @@
       <c r="F7" s="10">
         <v>4</v>
       </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
+    </row>
+    <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="10">
@@ -699,16 +711,15 @@
       <c r="F8" s="10">
         <v>5</v>
       </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
+    </row>
+    <row r="9" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="13">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="10">
@@ -717,18 +728,15 @@
       <c r="F9" s="10">
         <v>6</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
+    </row>
+    <row r="10" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="10">
@@ -737,16 +745,15 @@
       <c r="F10" s="10">
         <v>7</v>
       </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
+    </row>
+    <row r="11" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="10">
@@ -755,16 +762,15 @@
       <c r="F11" s="10">
         <v>8</v>
       </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
+    </row>
+    <row r="12" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="10">
@@ -773,16 +779,16 @@
       <c r="F12" s="10">
         <v>9</v>
       </c>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
         <v>10</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="10">
@@ -791,18 +797,15 @@
       <c r="F13" s="10">
         <v>10</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
+    </row>
+    <row r="14" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
         <v>11</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="10">
@@ -811,18 +814,15 @@
       <c r="F14" s="10">
         <v>11</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
+    </row>
+    <row r="15" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
         <v>12</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="10">
@@ -831,16 +831,15 @@
       <c r="F15" s="10">
         <v>12</v>
       </c>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
+    </row>
+    <row r="16" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="13">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="10">
@@ -849,16 +848,15 @@
       <c r="F16" s="10">
         <v>13</v>
       </c>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+    </row>
+    <row r="17" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="13">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="10">
@@ -867,16 +865,15 @@
       <c r="F17" s="10">
         <v>14</v>
       </c>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+    </row>
+    <row r="18" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="13">
         <v>15</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="10">
@@ -885,16 +882,15 @@
       <c r="F18" s="10">
         <v>15</v>
       </c>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8">
+    </row>
+    <row r="19" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13">
         <v>16</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="10">
@@ -903,16 +899,15 @@
       <c r="F19" s="10">
         <v>16</v>
       </c>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8">
+    </row>
+    <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13">
         <v>17</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="10">
@@ -921,16 +916,15 @@
       <c r="F20" s="10">
         <v>17</v>
       </c>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="8">
+    </row>
+    <row r="21" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13">
         <v>18</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="10">
@@ -939,16 +933,15 @@
       <c r="F21" s="10">
         <v>18</v>
       </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8">
+    </row>
+    <row r="22" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="13">
         <v>19</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="10">
@@ -957,16 +950,15 @@
       <c r="F22" s="10">
         <v>19</v>
       </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="8">
+    </row>
+    <row r="23" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13">
         <v>20</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="10">
@@ -975,16 +967,15 @@
       <c r="F23" s="10">
         <v>20</v>
       </c>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="8">
+    </row>
+    <row r="24" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="13">
         <v>21</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="10">
@@ -993,9 +984,8 @@
       <c r="F24" s="10">
         <v>21</v>
       </c>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1003,6 +993,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>